<commit_message>
Update film inspection system with additional forms and backend integration
- Update server.js with UC-18gsm-250W-BFQR export functionality
- Add UC-18gsm-210W-BFQR Excel template
- Update film inspection forms list with UC-18gsm-250W-BFQR integration
- Update film inspection list JavaScript with UC-18gsm-250W-BFQR routing and functionality
</commit_message>
<xml_diff>
--- a/backend/templates/UC-18gsm-210W-BFQR.xlsx
+++ b/backend/templates/UC-18gsm-210W-BFQR.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27932"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC4F90D-A6F4-4F76-9213-FCEA46EC1D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DF15C3-7F5C-4D09-B4D7-CADAA4084D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page1" sheetId="6" r:id="rId1"/>
@@ -31,6 +31,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -1869,6 +1872,50 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1915,88 +1962,161 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2022,181 +2142,214 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2257,156 +2410,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3072,7 +3075,7 @@
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3086,35 +3089,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="138" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="147"/>
-      <c r="G1" s="147"/>
-      <c r="H1" s="147"/>
-      <c r="I1" s="147"/>
-      <c r="J1" s="147"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="G1" s="138"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="138"/>
+      <c r="J1" s="138"/>
       <c r="K1" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="147" t="s">
+      <c r="A2" s="138" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="147"/>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
-      <c r="E2" s="147"/>
-      <c r="F2" s="147"/>
-      <c r="G2" s="147"/>
-      <c r="H2" s="147"/>
-      <c r="I2" s="147"/>
-      <c r="J2" s="147"/>
+      <c r="B2" s="138"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
       <c r="K2" s="4" t="s">
         <v>29</v>
       </c>
@@ -3135,12 +3138,12 @@
       <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:13" s="45" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="148" t="s">
+      <c r="A4" s="139" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="149"/>
-      <c r="C4" s="150"/>
-      <c r="D4" s="151"/>
+      <c r="B4" s="140"/>
+      <c r="C4" s="141"/>
+      <c r="D4" s="142"/>
       <c r="E4" s="9" t="s">
         <v>4</v>
       </c>
@@ -3152,19 +3155,19 @@
       <c r="I4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="139"/>
-      <c r="K4" s="140"/>
+      <c r="J4" s="153"/>
+      <c r="K4" s="154"/>
       <c r="M4" s="45" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="45" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="152" t="s">
+      <c r="A5" s="143" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="153"/>
-      <c r="C5" s="154"/>
-      <c r="D5" s="155"/>
+      <c r="B5" s="144"/>
+      <c r="C5" s="145"/>
+      <c r="D5" s="146"/>
       <c r="E5" s="13" t="s">
         <v>7</v>
       </c>
@@ -3176,64 +3179,64 @@
       <c r="I5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="141"/>
-      <c r="K5" s="142"/>
+      <c r="J5" s="155"/>
+      <c r="K5" s="156"/>
     </row>
     <row r="6" spans="1:13" s="45" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="156" t="s">
+      <c r="A6" s="161" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="157"/>
-      <c r="C6" s="158"/>
+      <c r="B6" s="162"/>
+      <c r="C6" s="163"/>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
       <c r="F6" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="G6" s="134"/>
-      <c r="H6" s="146"/>
-      <c r="I6" s="134"/>
-      <c r="J6" s="135"/>
-      <c r="K6" s="136"/>
+      <c r="G6" s="148"/>
+      <c r="H6" s="160"/>
+      <c r="I6" s="148"/>
+      <c r="J6" s="149"/>
+      <c r="K6" s="150"/>
     </row>
     <row r="7" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="159" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="137"/>
-      <c r="C7" s="137"/>
-      <c r="D7" s="137" t="s">
+      <c r="A7" s="164" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="151"/>
+      <c r="C7" s="151"/>
+      <c r="D7" s="151" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="137" t="s">
+      <c r="E7" s="151" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="137" t="s">
+      <c r="F7" s="151" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="143" t="s">
+      <c r="G7" s="157" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="143" t="s">
+      <c r="H7" s="157" t="s">
         <v>122</v>
       </c>
-      <c r="I7" s="137" t="s">
+      <c r="I7" s="151" t="s">
         <v>1</v>
       </c>
-      <c r="J7" s="137"/>
-      <c r="K7" s="138"/>
+      <c r="J7" s="151"/>
+      <c r="K7" s="152"/>
     </row>
     <row r="8" spans="1:13" s="5" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="160"/>
-      <c r="B8" s="145"/>
-      <c r="C8" s="145"/>
-      <c r="D8" s="145"/>
-      <c r="E8" s="145" t="s">
+      <c r="A8" s="165"/>
+      <c r="B8" s="159"/>
+      <c r="C8" s="159"/>
+      <c r="D8" s="159"/>
+      <c r="E8" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="145"/>
-      <c r="G8" s="144"/>
-      <c r="H8" s="144"/>
+      <c r="F8" s="159"/>
+      <c r="G8" s="158"/>
+      <c r="H8" s="158"/>
       <c r="I8" s="1" t="s">
         <v>10</v>
       </c>
@@ -3635,11 +3638,11 @@
       <c r="K38" s="28"/>
     </row>
     <row r="39" spans="1:14" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="167" t="s">
+      <c r="A39" s="133" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="168"/>
-      <c r="C39" s="169"/>
+      <c r="B39" s="134"/>
+      <c r="C39" s="135"/>
       <c r="D39" s="35" t="e">
         <f t="shared" ref="D39:K39" si="0">AVERAGE(D9:D38)</f>
         <v>#DIV/0!</v>
@@ -3674,11 +3677,11 @@
       </c>
     </row>
     <row r="40" spans="1:14" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="164" t="s">
+      <c r="A40" s="169" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="165"/>
-      <c r="C40" s="166"/>
+      <c r="B40" s="170"/>
+      <c r="C40" s="171"/>
       <c r="D40" s="38">
         <f t="shared" ref="D40:K40" si="1">MIN(D9:D38)</f>
         <v>0</v>
@@ -3713,11 +3716,11 @@
       </c>
     </row>
     <row r="41" spans="1:14" s="45" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="161" t="s">
+      <c r="A41" s="166" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="162"/>
-      <c r="C41" s="163"/>
+      <c r="B41" s="167"/>
+      <c r="C41" s="168"/>
       <c r="D41" s="41">
         <f t="shared" ref="D41:K41" si="2">MAX(D9:D38)</f>
         <v>0</v>
@@ -3758,8 +3761,8 @@
       <c r="A42" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="B42" s="170"/>
-      <c r="C42" s="170"/>
+      <c r="B42" s="136"/>
+      <c r="C42" s="136"/>
       <c r="D42" s="44" t="s">
         <v>22</v>
       </c>
@@ -3776,8 +3779,8 @@
     </row>
     <row r="43" spans="1:14" s="45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="50"/>
-      <c r="B43" s="171"/>
-      <c r="C43" s="171"/>
+      <c r="B43" s="137"/>
+      <c r="C43" s="137"/>
       <c r="D43" s="44"/>
       <c r="F43" s="46"/>
       <c r="G43" s="47"/>
@@ -3786,11 +3789,11 @@
       <c r="J43" s="51"/>
     </row>
     <row r="44" spans="1:14" s="45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="133" t="s">
+      <c r="A44" s="147" t="s">
         <v>21</v>
       </c>
-      <c r="B44" s="133"/>
-      <c r="C44" s="133"/>
+      <c r="B44" s="147"/>
+      <c r="C44" s="147"/>
       <c r="D44" s="44"/>
       <c r="E44" s="44"/>
       <c r="F44" s="47" t="s">
@@ -3802,11 +3805,11 @@
       <c r="H44" s="44"/>
     </row>
     <row r="45" spans="1:14" s="45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="133" t="s">
+      <c r="A45" s="147" t="s">
         <v>135</v>
       </c>
-      <c r="B45" s="133"/>
-      <c r="C45" s="133"/>
+      <c r="B45" s="147"/>
+      <c r="C45" s="147"/>
       <c r="D45" s="44"/>
       <c r="E45" s="44"/>
       <c r="F45" s="44"/>
@@ -3848,15 +3851,6 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="25">
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
     <mergeCell ref="A45:C45"/>
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="I7:K7"/>
@@ -3873,6 +3867,15 @@
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="A41:C41"/>
     <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <conditionalFormatting sqref="D9:D41">
@@ -3948,7 +3951,7 @@
   <dimension ref="A1:K60"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14:J14"/>
+      <selection activeCell="I17" sqref="I17:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3959,35 +3962,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="138" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="147"/>
-      <c r="G1" s="147"/>
-      <c r="H1" s="147"/>
-      <c r="I1" s="147"/>
-      <c r="J1" s="147"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="G1" s="138"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="138"/>
+      <c r="J1" s="138"/>
       <c r="K1" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="147" t="s">
+      <c r="A2" s="138" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="147"/>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
-      <c r="E2" s="147"/>
-      <c r="F2" s="147"/>
-      <c r="G2" s="147"/>
-      <c r="H2" s="147"/>
-      <c r="I2" s="147"/>
-      <c r="J2" s="147"/>
+      <c r="B2" s="138"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
       <c r="K2" s="4" t="s">
         <v>29</v>
       </c>
@@ -4008,18 +4011,18 @@
       <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:11" s="45" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="148" t="s">
+      <c r="A4" s="139" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="149">
+      <c r="B4" s="140">
         <f ca="1">Page2!B4:D4</f>
         <v>0</v>
       </c>
-      <c r="C4" s="196">
+      <c r="C4" s="195">
         <f>Page1!C4</f>
         <v>0</v>
       </c>
-      <c r="D4" s="193"/>
+      <c r="D4" s="196"/>
       <c r="E4" s="9" t="s">
         <v>4</v>
       </c>
@@ -4037,25 +4040,25 @@
       <c r="I4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="234">
+      <c r="J4" s="191">
         <f>Page2!K4</f>
         <v>0</v>
       </c>
-      <c r="K4" s="235"/>
+      <c r="K4" s="192"/>
     </row>
     <row r="5" spans="1:11" s="45" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="152" t="s">
+      <c r="A5" s="143" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="153">
+      <c r="B5" s="144">
         <f ca="1">Page2!B5:D5</f>
         <v>0</v>
       </c>
-      <c r="C5" s="154">
+      <c r="C5" s="145">
         <f>Page1!C5</f>
         <v>0</v>
       </c>
-      <c r="D5" s="155"/>
+      <c r="D5" s="146"/>
       <c r="E5" s="13" t="s">
         <v>7</v>
       </c>
@@ -4073,113 +4076,113 @@
       <c r="I5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="236">
+      <c r="J5" s="193">
         <f>Page2!K5</f>
         <v>0</v>
       </c>
-      <c r="K5" s="237"/>
+      <c r="K5" s="194"/>
     </row>
     <row r="6" spans="1:11" s="45" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="182" t="s">
+      <c r="A6" s="201" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="183"/>
-      <c r="C6" s="184"/>
-      <c r="D6" s="185"/>
-      <c r="E6" s="186"/>
-      <c r="F6" s="187"/>
-      <c r="G6" s="200"/>
-      <c r="H6" s="187"/>
-      <c r="I6" s="198"/>
-      <c r="J6" s="199"/>
+      <c r="B6" s="202"/>
+      <c r="C6" s="203"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="198"/>
+      <c r="F6" s="190"/>
+      <c r="G6" s="189"/>
+      <c r="H6" s="190"/>
+      <c r="I6" s="187"/>
+      <c r="J6" s="188"/>
       <c r="K6" s="56"/>
     </row>
     <row r="7" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="185" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="186"/>
-      <c r="C7" s="186"/>
-      <c r="D7" s="192" t="s">
+      <c r="A7" s="197" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="198"/>
+      <c r="C7" s="198"/>
+      <c r="D7" s="208" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="186"/>
-      <c r="F7" s="193"/>
-      <c r="G7" s="200" t="s">
+      <c r="E7" s="198"/>
+      <c r="F7" s="196"/>
+      <c r="G7" s="189" t="s">
         <v>126</v>
       </c>
-      <c r="H7" s="186"/>
-      <c r="I7" s="200" t="s">
+      <c r="H7" s="198"/>
+      <c r="I7" s="189" t="s">
         <v>136</v>
       </c>
-      <c r="J7" s="187"/>
-      <c r="K7" s="209" t="s">
+      <c r="J7" s="190"/>
+      <c r="K7" s="182" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="172"/>
-      <c r="B8" s="197"/>
-      <c r="C8" s="197"/>
-      <c r="D8" s="172" t="s">
+      <c r="A8" s="199"/>
+      <c r="B8" s="200"/>
+      <c r="C8" s="200"/>
+      <c r="D8" s="199" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="174" t="s">
+      <c r="E8" s="211" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="175" t="s">
+      <c r="F8" s="212" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="177"/>
-      <c r="H8" s="197"/>
-      <c r="I8" s="177" t="s">
+      <c r="G8" s="214"/>
+      <c r="H8" s="200"/>
+      <c r="I8" s="214" t="s">
         <v>137</v>
       </c>
-      <c r="J8" s="175"/>
-      <c r="K8" s="210"/>
+      <c r="J8" s="212"/>
+      <c r="K8" s="183"/>
     </row>
     <row r="9" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="172"/>
-      <c r="B9" s="197"/>
-      <c r="C9" s="197"/>
-      <c r="D9" s="172"/>
-      <c r="E9" s="143"/>
-      <c r="F9" s="175"/>
-      <c r="G9" s="177"/>
-      <c r="H9" s="197"/>
+      <c r="A9" s="199"/>
+      <c r="B9" s="200"/>
+      <c r="C9" s="200"/>
+      <c r="D9" s="199"/>
+      <c r="E9" s="157"/>
+      <c r="F9" s="212"/>
+      <c r="G9" s="214"/>
+      <c r="H9" s="200"/>
       <c r="I9" s="58" t="s">
         <v>123</v>
       </c>
       <c r="J9" s="59">
-        <v>250</v>
-      </c>
-      <c r="K9" s="210"/>
+        <v>210</v>
+      </c>
+      <c r="K9" s="183"/>
     </row>
     <row r="10" spans="1:11" s="5" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="172">
+      <c r="A10" s="199">
         <f>Page1!A9</f>
         <v>0</v>
       </c>
-      <c r="B10" s="197">
+      <c r="B10" s="200">
         <f>Page1!B9</f>
         <v>0</v>
       </c>
-      <c r="C10" s="197">
+      <c r="C10" s="200">
         <f>Page1!C9</f>
         <v>0</v>
       </c>
-      <c r="D10" s="173"/>
-      <c r="E10" s="144"/>
-      <c r="F10" s="176"/>
-      <c r="G10" s="201"/>
-      <c r="H10" s="202"/>
+      <c r="D10" s="225"/>
+      <c r="E10" s="158"/>
+      <c r="F10" s="213"/>
+      <c r="G10" s="219"/>
+      <c r="H10" s="220"/>
       <c r="I10" s="60" t="s">
         <v>124</v>
       </c>
       <c r="J10" s="61">
-        <v>253</v>
-      </c>
-      <c r="K10" s="211"/>
+        <v>213</v>
+      </c>
+      <c r="K10" s="184"/>
     </row>
     <row r="11" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="62">
@@ -4197,10 +4200,10 @@
       <c r="D11" s="65"/>
       <c r="E11" s="24"/>
       <c r="F11" s="24"/>
-      <c r="G11" s="221"/>
-      <c r="H11" s="221"/>
-      <c r="I11" s="203"/>
-      <c r="J11" s="204"/>
+      <c r="G11" s="176"/>
+      <c r="H11" s="176"/>
+      <c r="I11" s="221"/>
+      <c r="J11" s="222"/>
       <c r="K11" s="66"/>
     </row>
     <row r="12" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4219,10 +4222,10 @@
       <c r="D12" s="70"/>
       <c r="E12" s="25"/>
       <c r="F12" s="25"/>
-      <c r="G12" s="214"/>
-      <c r="H12" s="214"/>
-      <c r="I12" s="205"/>
-      <c r="J12" s="206"/>
+      <c r="G12" s="177"/>
+      <c r="H12" s="177"/>
+      <c r="I12" s="174"/>
+      <c r="J12" s="175"/>
       <c r="K12" s="71"/>
     </row>
     <row r="13" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4241,10 +4244,10 @@
       <c r="D13" s="70"/>
       <c r="E13" s="25"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="214"/>
-      <c r="H13" s="214"/>
-      <c r="I13" s="205"/>
-      <c r="J13" s="206"/>
+      <c r="G13" s="177"/>
+      <c r="H13" s="177"/>
+      <c r="I13" s="174"/>
+      <c r="J13" s="175"/>
       <c r="K13" s="71"/>
     </row>
     <row r="14" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4263,10 +4266,10 @@
       <c r="D14" s="70"/>
       <c r="E14" s="25"/>
       <c r="F14" s="25"/>
-      <c r="G14" s="214"/>
-      <c r="H14" s="214"/>
-      <c r="I14" s="205"/>
-      <c r="J14" s="206"/>
+      <c r="G14" s="177"/>
+      <c r="H14" s="177"/>
+      <c r="I14" s="174"/>
+      <c r="J14" s="175"/>
       <c r="K14" s="71"/>
     </row>
     <row r="15" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4285,10 +4288,10 @@
       <c r="D15" s="70"/>
       <c r="E15" s="25"/>
       <c r="F15" s="25"/>
-      <c r="G15" s="214"/>
-      <c r="H15" s="214"/>
-      <c r="I15" s="205"/>
-      <c r="J15" s="206"/>
+      <c r="G15" s="177"/>
+      <c r="H15" s="177"/>
+      <c r="I15" s="174"/>
+      <c r="J15" s="175"/>
       <c r="K15" s="71"/>
     </row>
     <row r="16" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4307,10 +4310,10 @@
       <c r="D16" s="65"/>
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
-      <c r="G16" s="221"/>
-      <c r="H16" s="221"/>
-      <c r="I16" s="205"/>
-      <c r="J16" s="206"/>
+      <c r="G16" s="176"/>
+      <c r="H16" s="176"/>
+      <c r="I16" s="174"/>
+      <c r="J16" s="175"/>
       <c r="K16" s="66"/>
     </row>
     <row r="17" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4329,10 +4332,10 @@
       <c r="D17" s="70"/>
       <c r="E17" s="25"/>
       <c r="F17" s="25"/>
-      <c r="G17" s="214"/>
-      <c r="H17" s="214"/>
-      <c r="I17" s="205"/>
-      <c r="J17" s="206"/>
+      <c r="G17" s="177"/>
+      <c r="H17" s="177"/>
+      <c r="I17" s="174"/>
+      <c r="J17" s="175"/>
       <c r="K17" s="71"/>
     </row>
     <row r="18" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4351,10 +4354,10 @@
       <c r="D18" s="70"/>
       <c r="E18" s="25"/>
       <c r="F18" s="25"/>
-      <c r="G18" s="214"/>
-      <c r="H18" s="214"/>
-      <c r="I18" s="205"/>
-      <c r="J18" s="206"/>
+      <c r="G18" s="177"/>
+      <c r="H18" s="177"/>
+      <c r="I18" s="174"/>
+      <c r="J18" s="175"/>
       <c r="K18" s="71"/>
     </row>
     <row r="19" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4373,10 +4376,10 @@
       <c r="D19" s="70"/>
       <c r="E19" s="25"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="214"/>
-      <c r="H19" s="214"/>
-      <c r="I19" s="205"/>
-      <c r="J19" s="206"/>
+      <c r="G19" s="177"/>
+      <c r="H19" s="177"/>
+      <c r="I19" s="174"/>
+      <c r="J19" s="175"/>
       <c r="K19" s="71"/>
     </row>
     <row r="20" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4395,10 +4398,10 @@
       <c r="D20" s="70"/>
       <c r="E20" s="25"/>
       <c r="F20" s="25"/>
-      <c r="G20" s="215"/>
-      <c r="H20" s="216"/>
-      <c r="I20" s="205"/>
-      <c r="J20" s="206"/>
+      <c r="G20" s="172"/>
+      <c r="H20" s="173"/>
+      <c r="I20" s="174"/>
+      <c r="J20" s="175"/>
       <c r="K20" s="71"/>
     </row>
     <row r="21" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4417,10 +4420,10 @@
       <c r="D21" s="70"/>
       <c r="E21" s="25"/>
       <c r="F21" s="25"/>
-      <c r="G21" s="215"/>
-      <c r="H21" s="216"/>
-      <c r="I21" s="205"/>
-      <c r="J21" s="206"/>
+      <c r="G21" s="172"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="174"/>
+      <c r="J21" s="175"/>
       <c r="K21" s="71"/>
     </row>
     <row r="22" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4439,10 +4442,10 @@
       <c r="D22" s="70"/>
       <c r="E22" s="25"/>
       <c r="F22" s="25"/>
-      <c r="G22" s="215"/>
-      <c r="H22" s="216"/>
-      <c r="I22" s="205"/>
-      <c r="J22" s="206"/>
+      <c r="G22" s="172"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="174"/>
+      <c r="J22" s="175"/>
       <c r="K22" s="71"/>
     </row>
     <row r="23" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4461,10 +4464,10 @@
       <c r="D23" s="70"/>
       <c r="E23" s="25"/>
       <c r="F23" s="25"/>
-      <c r="G23" s="215"/>
-      <c r="H23" s="216"/>
-      <c r="I23" s="205"/>
-      <c r="J23" s="206"/>
+      <c r="G23" s="172"/>
+      <c r="H23" s="173"/>
+      <c r="I23" s="174"/>
+      <c r="J23" s="175"/>
       <c r="K23" s="71"/>
     </row>
     <row r="24" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4483,10 +4486,10 @@
       <c r="D24" s="70"/>
       <c r="E24" s="25"/>
       <c r="F24" s="25"/>
-      <c r="G24" s="215"/>
-      <c r="H24" s="216"/>
-      <c r="I24" s="205"/>
-      <c r="J24" s="206"/>
+      <c r="G24" s="172"/>
+      <c r="H24" s="173"/>
+      <c r="I24" s="174"/>
+      <c r="J24" s="175"/>
       <c r="K24" s="71"/>
     </row>
     <row r="25" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4505,10 +4508,10 @@
       <c r="D25" s="70"/>
       <c r="E25" s="25"/>
       <c r="F25" s="25"/>
-      <c r="G25" s="215"/>
-      <c r="H25" s="216"/>
-      <c r="I25" s="205"/>
-      <c r="J25" s="206"/>
+      <c r="G25" s="172"/>
+      <c r="H25" s="173"/>
+      <c r="I25" s="174"/>
+      <c r="J25" s="175"/>
       <c r="K25" s="71"/>
     </row>
     <row r="26" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4527,10 +4530,10 @@
       <c r="D26" s="70"/>
       <c r="E26" s="25"/>
       <c r="F26" s="25"/>
-      <c r="G26" s="215"/>
-      <c r="H26" s="216"/>
-      <c r="I26" s="205"/>
-      <c r="J26" s="206"/>
+      <c r="G26" s="172"/>
+      <c r="H26" s="173"/>
+      <c r="I26" s="174"/>
+      <c r="J26" s="175"/>
       <c r="K26" s="71"/>
     </row>
     <row r="27" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4549,10 +4552,10 @@
       <c r="D27" s="70"/>
       <c r="E27" s="25"/>
       <c r="F27" s="25"/>
-      <c r="G27" s="215"/>
-      <c r="H27" s="216"/>
-      <c r="I27" s="205"/>
-      <c r="J27" s="206"/>
+      <c r="G27" s="172"/>
+      <c r="H27" s="173"/>
+      <c r="I27" s="174"/>
+      <c r="J27" s="175"/>
       <c r="K27" s="71"/>
     </row>
     <row r="28" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4571,10 +4574,10 @@
       <c r="D28" s="70"/>
       <c r="E28" s="25"/>
       <c r="F28" s="25"/>
-      <c r="G28" s="215"/>
-      <c r="H28" s="216"/>
-      <c r="I28" s="205"/>
-      <c r="J28" s="206"/>
+      <c r="G28" s="172"/>
+      <c r="H28" s="173"/>
+      <c r="I28" s="174"/>
+      <c r="J28" s="175"/>
       <c r="K28" s="71"/>
     </row>
     <row r="29" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4593,10 +4596,10 @@
       <c r="D29" s="70"/>
       <c r="E29" s="25"/>
       <c r="F29" s="25"/>
-      <c r="G29" s="215"/>
-      <c r="H29" s="216"/>
-      <c r="I29" s="205"/>
-      <c r="J29" s="206"/>
+      <c r="G29" s="172"/>
+      <c r="H29" s="173"/>
+      <c r="I29" s="174"/>
+      <c r="J29" s="175"/>
       <c r="K29" s="71"/>
     </row>
     <row r="30" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4615,10 +4618,10 @@
       <c r="D30" s="70"/>
       <c r="E30" s="25"/>
       <c r="F30" s="25"/>
-      <c r="G30" s="215"/>
-      <c r="H30" s="216"/>
-      <c r="I30" s="205"/>
-      <c r="J30" s="206"/>
+      <c r="G30" s="172"/>
+      <c r="H30" s="173"/>
+      <c r="I30" s="174"/>
+      <c r="J30" s="175"/>
       <c r="K30" s="71"/>
     </row>
     <row r="31" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4637,10 +4640,10 @@
       <c r="D31" s="70"/>
       <c r="E31" s="25"/>
       <c r="F31" s="25"/>
-      <c r="G31" s="215"/>
-      <c r="H31" s="216"/>
-      <c r="I31" s="205"/>
-      <c r="J31" s="206"/>
+      <c r="G31" s="172"/>
+      <c r="H31" s="173"/>
+      <c r="I31" s="174"/>
+      <c r="J31" s="175"/>
       <c r="K31" s="71"/>
     </row>
     <row r="32" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4659,10 +4662,10 @@
       <c r="D32" s="70"/>
       <c r="E32" s="25"/>
       <c r="F32" s="25"/>
-      <c r="G32" s="215"/>
-      <c r="H32" s="216"/>
-      <c r="I32" s="205"/>
-      <c r="J32" s="206"/>
+      <c r="G32" s="172"/>
+      <c r="H32" s="173"/>
+      <c r="I32" s="174"/>
+      <c r="J32" s="175"/>
       <c r="K32" s="71"/>
     </row>
     <row r="33" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4681,10 +4684,10 @@
       <c r="D33" s="70"/>
       <c r="E33" s="25"/>
       <c r="F33" s="25"/>
-      <c r="G33" s="215"/>
-      <c r="H33" s="216"/>
-      <c r="I33" s="205"/>
-      <c r="J33" s="206"/>
+      <c r="G33" s="172"/>
+      <c r="H33" s="173"/>
+      <c r="I33" s="174"/>
+      <c r="J33" s="175"/>
       <c r="K33" s="71"/>
     </row>
     <row r="34" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4703,10 +4706,10 @@
       <c r="D34" s="70"/>
       <c r="E34" s="25"/>
       <c r="F34" s="25"/>
-      <c r="G34" s="215"/>
-      <c r="H34" s="216"/>
-      <c r="I34" s="205"/>
-      <c r="J34" s="206"/>
+      <c r="G34" s="172"/>
+      <c r="H34" s="173"/>
+      <c r="I34" s="174"/>
+      <c r="J34" s="175"/>
       <c r="K34" s="71"/>
     </row>
     <row r="35" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4725,10 +4728,10 @@
       <c r="D35" s="70"/>
       <c r="E35" s="25"/>
       <c r="F35" s="25"/>
-      <c r="G35" s="215"/>
-      <c r="H35" s="216"/>
-      <c r="I35" s="205"/>
-      <c r="J35" s="206"/>
+      <c r="G35" s="172"/>
+      <c r="H35" s="173"/>
+      <c r="I35" s="174"/>
+      <c r="J35" s="175"/>
       <c r="K35" s="71"/>
     </row>
     <row r="36" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4747,10 +4750,10 @@
       <c r="D36" s="70"/>
       <c r="E36" s="25"/>
       <c r="F36" s="25"/>
-      <c r="G36" s="215"/>
-      <c r="H36" s="216"/>
-      <c r="I36" s="205"/>
-      <c r="J36" s="206"/>
+      <c r="G36" s="172"/>
+      <c r="H36" s="173"/>
+      <c r="I36" s="174"/>
+      <c r="J36" s="175"/>
       <c r="K36" s="71"/>
     </row>
     <row r="37" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4769,10 +4772,10 @@
       <c r="D37" s="70"/>
       <c r="E37" s="25"/>
       <c r="F37" s="25"/>
-      <c r="G37" s="215"/>
-      <c r="H37" s="216"/>
-      <c r="I37" s="205"/>
-      <c r="J37" s="206"/>
+      <c r="G37" s="172"/>
+      <c r="H37" s="173"/>
+      <c r="I37" s="174"/>
+      <c r="J37" s="175"/>
       <c r="K37" s="71"/>
     </row>
     <row r="38" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4791,10 +4794,10 @@
       <c r="D38" s="70"/>
       <c r="E38" s="25"/>
       <c r="F38" s="25"/>
-      <c r="G38" s="215"/>
-      <c r="H38" s="216"/>
-      <c r="I38" s="205"/>
-      <c r="J38" s="206"/>
+      <c r="G38" s="172"/>
+      <c r="H38" s="173"/>
+      <c r="I38" s="174"/>
+      <c r="J38" s="175"/>
       <c r="K38" s="71"/>
     </row>
     <row r="39" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4813,10 +4816,10 @@
       <c r="D39" s="70"/>
       <c r="E39" s="25"/>
       <c r="F39" s="25"/>
-      <c r="G39" s="215"/>
-      <c r="H39" s="216"/>
-      <c r="I39" s="205"/>
-      <c r="J39" s="206"/>
+      <c r="G39" s="172"/>
+      <c r="H39" s="173"/>
+      <c r="I39" s="174"/>
+      <c r="J39" s="175"/>
       <c r="K39" s="71"/>
     </row>
     <row r="40" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4835,18 +4838,18 @@
       <c r="D40" s="70"/>
       <c r="E40" s="25"/>
       <c r="F40" s="25"/>
-      <c r="G40" s="214"/>
-      <c r="H40" s="214"/>
-      <c r="I40" s="205"/>
-      <c r="J40" s="206"/>
+      <c r="G40" s="177"/>
+      <c r="H40" s="177"/>
+      <c r="I40" s="174"/>
+      <c r="J40" s="175"/>
       <c r="K40" s="71"/>
     </row>
     <row r="41" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="194" t="s">
+      <c r="A41" s="209" t="s">
         <v>26</v>
       </c>
-      <c r="B41" s="195"/>
-      <c r="C41" s="195"/>
+      <c r="B41" s="210"/>
+      <c r="C41" s="210"/>
       <c r="D41" s="79" t="e">
         <f>AVERAGE(D11:D40)</f>
         <v>#DIV/0!</v>
@@ -4859,27 +4862,27 @@
         <f>AVERAGE(F11:F40)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G41" s="219" t="e">
+      <c r="G41" s="180" t="e">
         <f>AVERAGE(G11:H40)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H41" s="220"/>
-      <c r="I41" s="207" t="e">
+      <c r="H41" s="181"/>
+      <c r="I41" s="223" t="e">
         <f>AVERAGE(I11:J40)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J41" s="208"/>
+      <c r="J41" s="224"/>
       <c r="K41" s="37" t="e">
         <f>AVERAGE(K11:K40)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="42" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="188" t="s">
+      <c r="A42" s="204" t="s">
         <v>31</v>
       </c>
-      <c r="B42" s="189"/>
-      <c r="C42" s="189"/>
+      <c r="B42" s="205"/>
+      <c r="C42" s="205"/>
       <c r="D42" s="80">
         <f>MIN(D11:D40)</f>
         <v>0</v>
@@ -4892,27 +4895,27 @@
         <f>MIN(F11:F40)</f>
         <v>0</v>
       </c>
-      <c r="G42" s="217">
+      <c r="G42" s="178">
         <f>MIN(G11:H40)</f>
         <v>0</v>
       </c>
-      <c r="H42" s="218"/>
-      <c r="I42" s="212">
+      <c r="H42" s="179"/>
+      <c r="I42" s="185">
         <f>MIN(I11:J40)</f>
         <v>0</v>
       </c>
-      <c r="J42" s="213"/>
+      <c r="J42" s="186"/>
       <c r="K42" s="40">
         <f>MIN(K11:K40)</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:11" s="5" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="190" t="s">
+      <c r="A43" s="206" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="191"/>
-      <c r="C43" s="191"/>
+      <c r="B43" s="207"/>
+      <c r="C43" s="207"/>
       <c r="D43" s="81">
         <f>MAX(D11:D40)</f>
         <v>0</v>
@@ -4925,16 +4928,16 @@
         <f>MAX(F11:F40)</f>
         <v>0</v>
       </c>
-      <c r="G43" s="178">
+      <c r="G43" s="215">
         <f>MAX(G11:H40)</f>
         <v>0</v>
       </c>
-      <c r="H43" s="179"/>
-      <c r="I43" s="180">
+      <c r="H43" s="216"/>
+      <c r="I43" s="217">
         <f>MAX(I11:J40)</f>
         <v>0</v>
       </c>
-      <c r="J43" s="181"/>
+      <c r="J43" s="218"/>
       <c r="K43" s="83">
         <f>MAX(K11:K40)</f>
         <v>0</v>
@@ -4944,8 +4947,8 @@
       <c r="A44" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="B44" s="170"/>
-      <c r="C44" s="170"/>
+      <c r="B44" s="136"/>
+      <c r="C44" s="136"/>
       <c r="D44" s="44" t="s">
         <v>22</v>
       </c>
@@ -4962,8 +4965,8 @@
     </row>
     <row r="45" spans="1:11" s="45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="50"/>
-      <c r="B45" s="171"/>
-      <c r="C45" s="171"/>
+      <c r="B45" s="137"/>
+      <c r="C45" s="137"/>
       <c r="D45" s="44"/>
       <c r="F45" s="46"/>
       <c r="G45" s="47"/>
@@ -4972,11 +4975,11 @@
       <c r="J45" s="51"/>
     </row>
     <row r="46" spans="1:11" s="45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="133" t="s">
+      <c r="A46" s="147" t="s">
         <v>21</v>
       </c>
-      <c r="B46" s="133"/>
-      <c r="C46" s="133"/>
+      <c r="B46" s="147"/>
+      <c r="C46" s="147"/>
       <c r="D46" s="44"/>
       <c r="E46" s="44"/>
       <c r="F46" s="47" t="s">
@@ -4989,11 +4992,11 @@
       <c r="H46" s="44"/>
     </row>
     <row r="47" spans="1:11" s="45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="133" t="s">
+      <c r="A47" s="147" t="s">
         <v>135</v>
       </c>
-      <c r="B47" s="133"/>
-      <c r="C47" s="133"/>
+      <c r="B47" s="147"/>
+      <c r="C47" s="147"/>
       <c r="D47" s="44"/>
       <c r="E47" s="44"/>
       <c r="F47" s="44"/>
@@ -5048,28 +5051,62 @@
     </row>
   </sheetData>
   <mergeCells count="94">
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="G7:H10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="K7:K10"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A7:C10"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="I38:J38"/>
     <mergeCell ref="I40:J40"/>
     <mergeCell ref="G40:H40"/>
     <mergeCell ref="I15:J15"/>
@@ -5086,62 +5123,28 @@
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="G39:H39"/>
     <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="K7:K10"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A7:C10"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="G7:H10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="I31:J31"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <conditionalFormatting sqref="D11:D43">
@@ -5202,35 +5205,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="138" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="147"/>
-      <c r="G1" s="147"/>
-      <c r="H1" s="147"/>
-      <c r="I1" s="147"/>
-      <c r="J1" s="147"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="G1" s="138"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="138"/>
+      <c r="J1" s="138"/>
       <c r="K1" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="147" t="s">
+      <c r="A2" s="138" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="147"/>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
-      <c r="E2" s="147"/>
-      <c r="F2" s="147"/>
-      <c r="G2" s="147"/>
-      <c r="H2" s="147"/>
-      <c r="I2" s="147"/>
-      <c r="J2" s="147"/>
+      <c r="B2" s="138"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
       <c r="K2" s="4" t="s">
         <v>29</v>
       </c>
@@ -5251,18 +5254,18 @@
       <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:11" s="45" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="148" t="s">
+      <c r="A4" s="139" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="149">
+      <c r="B4" s="140">
         <f ca="1">Page2!B4:D4</f>
         <v>0</v>
       </c>
-      <c r="C4" s="196">
+      <c r="C4" s="195">
         <f>Page1!C4</f>
         <v>0</v>
       </c>
-      <c r="D4" s="193"/>
+      <c r="D4" s="196"/>
       <c r="E4" s="9" t="s">
         <v>4</v>
       </c>
@@ -5280,25 +5283,25 @@
       <c r="I4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="234">
+      <c r="J4" s="191">
         <f>Page2!K4</f>
         <v>0</v>
       </c>
-      <c r="K4" s="235"/>
+      <c r="K4" s="192"/>
     </row>
     <row r="5" spans="1:11" s="45" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="152" t="s">
+      <c r="A5" s="143" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="153">
+      <c r="B5" s="144">
         <f ca="1">Page2!B5:D5</f>
         <v>0</v>
       </c>
-      <c r="C5" s="154">
+      <c r="C5" s="145">
         <f>Page1!C5</f>
         <v>0</v>
       </c>
-      <c r="D5" s="155"/>
+      <c r="D5" s="146"/>
       <c r="E5" s="13" t="s">
         <v>7</v>
       </c>
@@ -5316,79 +5319,79 @@
       <c r="I5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="236">
+      <c r="J5" s="193">
         <f>Page2!K5</f>
         <v>0</v>
       </c>
-      <c r="K5" s="237"/>
+      <c r="K5" s="194"/>
     </row>
     <row r="6" spans="1:11" s="45" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="230" t="s">
+      <c r="A6" s="229" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="231"/>
-      <c r="C6" s="232"/>
-      <c r="D6" s="233"/>
-      <c r="E6" s="135"/>
-      <c r="F6" s="135"/>
-      <c r="G6" s="146"/>
+      <c r="B6" s="230"/>
+      <c r="C6" s="231"/>
+      <c r="D6" s="232"/>
+      <c r="E6" s="149"/>
+      <c r="F6" s="149"/>
+      <c r="G6" s="160"/>
       <c r="H6" s="85"/>
-      <c r="I6" s="185"/>
-      <c r="J6" s="186"/>
-      <c r="K6" s="209"/>
+      <c r="I6" s="197"/>
+      <c r="J6" s="198"/>
+      <c r="K6" s="182"/>
     </row>
     <row r="7" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="185" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="186"/>
-      <c r="C7" s="186"/>
-      <c r="D7" s="192" t="s">
+      <c r="A7" s="197" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="198"/>
+      <c r="C7" s="198"/>
+      <c r="D7" s="208" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="222"/>
-      <c r="F7" s="222"/>
-      <c r="G7" s="193"/>
-      <c r="H7" s="227" t="s">
+      <c r="E7" s="233"/>
+      <c r="F7" s="233"/>
+      <c r="G7" s="196"/>
+      <c r="H7" s="226" t="s">
         <v>127</v>
       </c>
-      <c r="I7" s="172"/>
-      <c r="J7" s="197"/>
-      <c r="K7" s="210"/>
+      <c r="I7" s="199"/>
+      <c r="J7" s="200"/>
+      <c r="K7" s="183"/>
     </row>
     <row r="8" spans="1:11" s="5" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="172"/>
-      <c r="B8" s="197"/>
-      <c r="C8" s="197"/>
-      <c r="D8" s="225" t="s">
+      <c r="A8" s="199"/>
+      <c r="B8" s="200"/>
+      <c r="C8" s="200"/>
+      <c r="D8" s="236" t="s">
         <v>130</v>
       </c>
-      <c r="E8" s="174" t="s">
+      <c r="E8" s="211" t="s">
         <v>131</v>
       </c>
-      <c r="F8" s="174" t="s">
+      <c r="F8" s="211" t="s">
         <v>132</v>
       </c>
-      <c r="G8" s="174" t="s">
+      <c r="G8" s="211" t="s">
         <v>129</v>
       </c>
-      <c r="H8" s="228"/>
-      <c r="I8" s="172"/>
-      <c r="J8" s="197"/>
-      <c r="K8" s="210"/>
+      <c r="H8" s="227"/>
+      <c r="I8" s="199"/>
+      <c r="J8" s="200"/>
+      <c r="K8" s="183"/>
     </row>
     <row r="9" spans="1:11" s="5" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="172"/>
-      <c r="B9" s="197"/>
-      <c r="C9" s="197"/>
-      <c r="D9" s="226"/>
-      <c r="E9" s="144"/>
-      <c r="F9" s="144"/>
-      <c r="G9" s="144"/>
-      <c r="H9" s="229"/>
-      <c r="I9" s="172"/>
-      <c r="J9" s="197"/>
-      <c r="K9" s="210"/>
+      <c r="A9" s="199"/>
+      <c r="B9" s="200"/>
+      <c r="C9" s="200"/>
+      <c r="D9" s="237"/>
+      <c r="E9" s="158"/>
+      <c r="F9" s="158"/>
+      <c r="G9" s="158"/>
+      <c r="H9" s="228"/>
+      <c r="I9" s="199"/>
+      <c r="J9" s="200"/>
+      <c r="K9" s="183"/>
     </row>
     <row r="10" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="62">
@@ -5408,9 +5411,9 @@
       <c r="F10" s="23"/>
       <c r="G10" s="87"/>
       <c r="H10" s="88"/>
-      <c r="I10" s="172"/>
-      <c r="J10" s="197"/>
-      <c r="K10" s="210"/>
+      <c r="I10" s="199"/>
+      <c r="J10" s="200"/>
+      <c r="K10" s="183"/>
     </row>
     <row r="11" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="67">
@@ -5430,9 +5433,9 @@
       <c r="F11" s="26"/>
       <c r="G11" s="90"/>
       <c r="H11" s="91"/>
-      <c r="I11" s="172"/>
-      <c r="J11" s="197"/>
-      <c r="K11" s="210"/>
+      <c r="I11" s="199"/>
+      <c r="J11" s="200"/>
+      <c r="K11" s="183"/>
     </row>
     <row r="12" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="67">
@@ -5452,9 +5455,9 @@
       <c r="F12" s="26"/>
       <c r="G12" s="90"/>
       <c r="H12" s="91"/>
-      <c r="I12" s="172"/>
-      <c r="J12" s="197"/>
-      <c r="K12" s="210"/>
+      <c r="I12" s="199"/>
+      <c r="J12" s="200"/>
+      <c r="K12" s="183"/>
     </row>
     <row r="13" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="67">
@@ -5474,9 +5477,9 @@
       <c r="F13" s="23"/>
       <c r="G13" s="87"/>
       <c r="H13" s="91"/>
-      <c r="I13" s="172"/>
-      <c r="J13" s="197"/>
-      <c r="K13" s="210"/>
+      <c r="I13" s="199"/>
+      <c r="J13" s="200"/>
+      <c r="K13" s="183"/>
     </row>
     <row r="14" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="67">
@@ -5496,9 +5499,9 @@
       <c r="F14" s="26"/>
       <c r="G14" s="90"/>
       <c r="H14" s="91"/>
-      <c r="I14" s="172"/>
-      <c r="J14" s="197"/>
-      <c r="K14" s="210"/>
+      <c r="I14" s="199"/>
+      <c r="J14" s="200"/>
+      <c r="K14" s="183"/>
     </row>
     <row r="15" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="67">
@@ -5518,9 +5521,9 @@
       <c r="F15" s="26"/>
       <c r="G15" s="90"/>
       <c r="H15" s="91"/>
-      <c r="I15" s="172"/>
-      <c r="J15" s="197"/>
-      <c r="K15" s="210"/>
+      <c r="I15" s="199"/>
+      <c r="J15" s="200"/>
+      <c r="K15" s="183"/>
     </row>
     <row r="16" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="67">
@@ -5540,9 +5543,9 @@
       <c r="F16" s="26"/>
       <c r="G16" s="90"/>
       <c r="H16" s="91"/>
-      <c r="I16" s="172"/>
-      <c r="J16" s="197"/>
-      <c r="K16" s="210"/>
+      <c r="I16" s="199"/>
+      <c r="J16" s="200"/>
+      <c r="K16" s="183"/>
     </row>
     <row r="17" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="67">
@@ -5562,9 +5565,9 @@
       <c r="F17" s="26"/>
       <c r="G17" s="90"/>
       <c r="H17" s="91"/>
-      <c r="I17" s="172"/>
-      <c r="J17" s="197"/>
-      <c r="K17" s="210"/>
+      <c r="I17" s="199"/>
+      <c r="J17" s="200"/>
+      <c r="K17" s="183"/>
     </row>
     <row r="18" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="67">
@@ -5584,9 +5587,9 @@
       <c r="F18" s="26"/>
       <c r="G18" s="90"/>
       <c r="H18" s="91"/>
-      <c r="I18" s="172"/>
-      <c r="J18" s="197"/>
-      <c r="K18" s="210"/>
+      <c r="I18" s="199"/>
+      <c r="J18" s="200"/>
+      <c r="K18" s="183"/>
     </row>
     <row r="19" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="67">
@@ -5606,9 +5609,9 @@
       <c r="F19" s="26"/>
       <c r="G19" s="90"/>
       <c r="H19" s="91"/>
-      <c r="I19" s="172"/>
-      <c r="J19" s="197"/>
-      <c r="K19" s="210"/>
+      <c r="I19" s="199"/>
+      <c r="J19" s="200"/>
+      <c r="K19" s="183"/>
     </row>
     <row r="20" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="75">
@@ -5628,9 +5631,9 @@
       <c r="F20" s="26"/>
       <c r="G20" s="90"/>
       <c r="H20" s="91"/>
-      <c r="I20" s="172"/>
-      <c r="J20" s="197"/>
-      <c r="K20" s="210"/>
+      <c r="I20" s="199"/>
+      <c r="J20" s="200"/>
+      <c r="K20" s="183"/>
     </row>
     <row r="21" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="67">
@@ -5650,9 +5653,9 @@
       <c r="F21" s="26"/>
       <c r="G21" s="90"/>
       <c r="H21" s="91"/>
-      <c r="I21" s="172"/>
-      <c r="J21" s="197"/>
-      <c r="K21" s="210"/>
+      <c r="I21" s="199"/>
+      <c r="J21" s="200"/>
+      <c r="K21" s="183"/>
     </row>
     <row r="22" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="67">
@@ -5672,9 +5675,9 @@
       <c r="F22" s="26"/>
       <c r="G22" s="90"/>
       <c r="H22" s="91"/>
-      <c r="I22" s="172"/>
-      <c r="J22" s="197"/>
-      <c r="K22" s="210"/>
+      <c r="I22" s="199"/>
+      <c r="J22" s="200"/>
+      <c r="K22" s="183"/>
     </row>
     <row r="23" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="67">
@@ -5694,9 +5697,9 @@
       <c r="F23" s="26"/>
       <c r="G23" s="90"/>
       <c r="H23" s="91"/>
-      <c r="I23" s="172"/>
-      <c r="J23" s="197"/>
-      <c r="K23" s="210"/>
+      <c r="I23" s="199"/>
+      <c r="J23" s="200"/>
+      <c r="K23" s="183"/>
     </row>
     <row r="24" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="67">
@@ -5716,9 +5719,9 @@
       <c r="F24" s="26"/>
       <c r="G24" s="90"/>
       <c r="H24" s="91"/>
-      <c r="I24" s="172"/>
-      <c r="J24" s="197"/>
-      <c r="K24" s="210"/>
+      <c r="I24" s="199"/>
+      <c r="J24" s="200"/>
+      <c r="K24" s="183"/>
     </row>
     <row r="25" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="67">
@@ -5738,9 +5741,9 @@
       <c r="F25" s="26"/>
       <c r="G25" s="90"/>
       <c r="H25" s="91"/>
-      <c r="I25" s="172"/>
-      <c r="J25" s="197"/>
-      <c r="K25" s="210"/>
+      <c r="I25" s="199"/>
+      <c r="J25" s="200"/>
+      <c r="K25" s="183"/>
     </row>
     <row r="26" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="67">
@@ -5760,9 +5763,9 @@
       <c r="F26" s="26"/>
       <c r="G26" s="90"/>
       <c r="H26" s="91"/>
-      <c r="I26" s="172"/>
-      <c r="J26" s="197"/>
-      <c r="K26" s="210"/>
+      <c r="I26" s="199"/>
+      <c r="J26" s="200"/>
+      <c r="K26" s="183"/>
     </row>
     <row r="27" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="67">
@@ -5782,9 +5785,9 @@
       <c r="F27" s="26"/>
       <c r="G27" s="90"/>
       <c r="H27" s="91"/>
-      <c r="I27" s="172"/>
-      <c r="J27" s="197"/>
-      <c r="K27" s="210"/>
+      <c r="I27" s="199"/>
+      <c r="J27" s="200"/>
+      <c r="K27" s="183"/>
     </row>
     <row r="28" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="67">
@@ -5804,9 +5807,9 @@
       <c r="F28" s="26"/>
       <c r="G28" s="90"/>
       <c r="H28" s="91"/>
-      <c r="I28" s="172"/>
-      <c r="J28" s="197"/>
-      <c r="K28" s="210"/>
+      <c r="I28" s="199"/>
+      <c r="J28" s="200"/>
+      <c r="K28" s="183"/>
     </row>
     <row r="29" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="67">
@@ -5826,9 +5829,9 @@
       <c r="F29" s="26"/>
       <c r="G29" s="90"/>
       <c r="H29" s="91"/>
-      <c r="I29" s="172"/>
-      <c r="J29" s="197"/>
-      <c r="K29" s="210"/>
+      <c r="I29" s="199"/>
+      <c r="J29" s="200"/>
+      <c r="K29" s="183"/>
     </row>
     <row r="30" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="75">
@@ -5848,9 +5851,9 @@
       <c r="F30" s="26"/>
       <c r="G30" s="90"/>
       <c r="H30" s="91"/>
-      <c r="I30" s="172"/>
-      <c r="J30" s="197"/>
-      <c r="K30" s="210"/>
+      <c r="I30" s="199"/>
+      <c r="J30" s="200"/>
+      <c r="K30" s="183"/>
     </row>
     <row r="31" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="67">
@@ -5870,9 +5873,9 @@
       <c r="F31" s="26"/>
       <c r="G31" s="90"/>
       <c r="H31" s="91"/>
-      <c r="I31" s="172"/>
-      <c r="J31" s="197"/>
-      <c r="K31" s="210"/>
+      <c r="I31" s="199"/>
+      <c r="J31" s="200"/>
+      <c r="K31" s="183"/>
     </row>
     <row r="32" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="67">
@@ -5892,9 +5895,9 @@
       <c r="F32" s="26"/>
       <c r="G32" s="90"/>
       <c r="H32" s="91"/>
-      <c r="I32" s="172"/>
-      <c r="J32" s="197"/>
-      <c r="K32" s="210"/>
+      <c r="I32" s="199"/>
+      <c r="J32" s="200"/>
+      <c r="K32" s="183"/>
     </row>
     <row r="33" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="67">
@@ -5914,9 +5917,9 @@
       <c r="F33" s="26"/>
       <c r="G33" s="90"/>
       <c r="H33" s="91"/>
-      <c r="I33" s="172"/>
-      <c r="J33" s="197"/>
-      <c r="K33" s="210"/>
+      <c r="I33" s="199"/>
+      <c r="J33" s="200"/>
+      <c r="K33" s="183"/>
     </row>
     <row r="34" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="67">
@@ -5936,9 +5939,9 @@
       <c r="F34" s="26"/>
       <c r="G34" s="90"/>
       <c r="H34" s="91"/>
-      <c r="I34" s="172"/>
-      <c r="J34" s="197"/>
-      <c r="K34" s="210"/>
+      <c r="I34" s="199"/>
+      <c r="J34" s="200"/>
+      <c r="K34" s="183"/>
     </row>
     <row r="35" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="67">
@@ -5958,9 +5961,9 @@
       <c r="F35" s="26"/>
       <c r="G35" s="90"/>
       <c r="H35" s="91"/>
-      <c r="I35" s="172"/>
-      <c r="J35" s="197"/>
-      <c r="K35" s="210"/>
+      <c r="I35" s="199"/>
+      <c r="J35" s="200"/>
+      <c r="K35" s="183"/>
     </row>
     <row r="36" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="67">
@@ -5980,9 +5983,9 @@
       <c r="F36" s="26"/>
       <c r="G36" s="90"/>
       <c r="H36" s="91"/>
-      <c r="I36" s="172"/>
-      <c r="J36" s="197"/>
-      <c r="K36" s="210"/>
+      <c r="I36" s="199"/>
+      <c r="J36" s="200"/>
+      <c r="K36" s="183"/>
     </row>
     <row r="37" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="67">
@@ -6002,9 +6005,9 @@
       <c r="F37" s="26"/>
       <c r="G37" s="90"/>
       <c r="H37" s="91"/>
-      <c r="I37" s="172"/>
-      <c r="J37" s="197"/>
-      <c r="K37" s="210"/>
+      <c r="I37" s="199"/>
+      <c r="J37" s="200"/>
+      <c r="K37" s="183"/>
     </row>
     <row r="38" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="67">
@@ -6024,9 +6027,9 @@
       <c r="F38" s="26"/>
       <c r="G38" s="90"/>
       <c r="H38" s="91"/>
-      <c r="I38" s="172"/>
-      <c r="J38" s="197"/>
-      <c r="K38" s="210"/>
+      <c r="I38" s="199"/>
+      <c r="J38" s="200"/>
+      <c r="K38" s="183"/>
     </row>
     <row r="39" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="76">
@@ -6046,16 +6049,16 @@
       <c r="F39" s="26"/>
       <c r="G39" s="90"/>
       <c r="H39" s="91"/>
-      <c r="I39" s="172"/>
-      <c r="J39" s="197"/>
-      <c r="K39" s="210"/>
+      <c r="I39" s="199"/>
+      <c r="J39" s="200"/>
+      <c r="K39" s="183"/>
     </row>
     <row r="40" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="223" t="s">
+      <c r="A40" s="234" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="224"/>
-      <c r="C40" s="224"/>
+      <c r="B40" s="235"/>
+      <c r="C40" s="235"/>
       <c r="D40" s="92" t="e">
         <f>AVERAGE(D10:D39)</f>
         <v>#DIV/0!</v>
@@ -6076,16 +6079,16 @@
         <f>AVERAGE(H10:H39)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I40" s="197"/>
-      <c r="J40" s="197"/>
-      <c r="K40" s="210"/>
+      <c r="I40" s="200"/>
+      <c r="J40" s="200"/>
+      <c r="K40" s="183"/>
     </row>
     <row r="41" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="188" t="s">
+      <c r="A41" s="204" t="s">
         <v>31</v>
       </c>
-      <c r="B41" s="189"/>
-      <c r="C41" s="189"/>
+      <c r="B41" s="205"/>
+      <c r="C41" s="205"/>
       <c r="D41" s="94">
         <f>MIN(D10:D39)</f>
         <v>0</v>
@@ -6106,16 +6109,16 @@
         <f>MIN(H10:H39)</f>
         <v>0</v>
       </c>
-      <c r="I41" s="197"/>
-      <c r="J41" s="197"/>
-      <c r="K41" s="210"/>
+      <c r="I41" s="200"/>
+      <c r="J41" s="200"/>
+      <c r="K41" s="183"/>
     </row>
     <row r="42" spans="1:11" s="5" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="190" t="s">
+      <c r="A42" s="206" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="191"/>
-      <c r="C42" s="191"/>
+      <c r="B42" s="207"/>
+      <c r="C42" s="207"/>
       <c r="D42" s="96">
         <f>MAX(D10:D39)</f>
         <v>0</v>
@@ -6136,16 +6139,16 @@
         <f>MAX(H10:H39)</f>
         <v>0</v>
       </c>
-      <c r="I42" s="202"/>
-      <c r="J42" s="202"/>
-      <c r="K42" s="211"/>
+      <c r="I42" s="220"/>
+      <c r="J42" s="220"/>
+      <c r="K42" s="184"/>
     </row>
     <row r="43" spans="1:11" s="45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="B43" s="170"/>
-      <c r="C43" s="170"/>
+      <c r="B43" s="136"/>
+      <c r="C43" s="136"/>
       <c r="D43" s="44" t="s">
         <v>22</v>
       </c>
@@ -6162,8 +6165,8 @@
     </row>
     <row r="44" spans="1:11" s="45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="50"/>
-      <c r="B44" s="171"/>
-      <c r="C44" s="171"/>
+      <c r="B44" s="137"/>
+      <c r="C44" s="137"/>
       <c r="D44" s="44"/>
       <c r="F44" s="46"/>
       <c r="G44" s="47"/>
@@ -6172,11 +6175,11 @@
       <c r="J44" s="51"/>
     </row>
     <row r="45" spans="1:11" s="45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="133" t="s">
+      <c r="A45" s="147" t="s">
         <v>21</v>
       </c>
-      <c r="B45" s="133"/>
-      <c r="C45" s="133"/>
+      <c r="B45" s="147"/>
+      <c r="C45" s="147"/>
       <c r="D45" s="44"/>
       <c r="E45" s="44"/>
       <c r="F45" s="47" t="s">
@@ -6189,11 +6192,11 @@
       <c r="H45" s="44"/>
     </row>
     <row r="46" spans="1:11" s="45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="133" t="s">
+      <c r="A46" s="147" t="s">
         <v>135</v>
       </c>
-      <c r="B46" s="133"/>
-      <c r="C46" s="133"/>
+      <c r="B46" s="147"/>
+      <c r="C46" s="147"/>
       <c r="D46" s="44"/>
       <c r="E46" s="44"/>
       <c r="F46" s="44"/>
@@ -6218,18 +6221,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="I6:K42"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
     <mergeCell ref="A46:C46"/>
     <mergeCell ref="A45:C45"/>
     <mergeCell ref="D7:G7"/>
@@ -6243,6 +6234,18 @@
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
+    <mergeCell ref="I6:K42"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <conditionalFormatting sqref="D10:D42">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="notBetween">
@@ -6294,15 +6297,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="301" t="s">
+      <c r="A1" s="238" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="302"/>
-      <c r="C1" s="302"/>
-      <c r="D1" s="302"/>
-      <c r="E1" s="302"/>
-      <c r="F1" s="302"/>
-      <c r="G1" s="303"/>
+      <c r="B1" s="239"/>
+      <c r="C1" s="239"/>
+      <c r="D1" s="239"/>
+      <c r="E1" s="239"/>
+      <c r="F1" s="239"/>
+      <c r="G1" s="240"/>
     </row>
     <row r="2" spans="1:7" s="99" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="100"/>
@@ -6316,37 +6319,37 @@
       </c>
     </row>
     <row r="3" spans="1:7" s="99" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="242" t="s">
+      <c r="A3" s="292" t="s">
         <v>141</v>
       </c>
-      <c r="B3" s="243"/>
-      <c r="C3" s="243"/>
-      <c r="D3" s="243"/>
-      <c r="E3" s="243"/>
-      <c r="F3" s="243"/>
-      <c r="G3" s="244"/>
+      <c r="B3" s="293"/>
+      <c r="C3" s="293"/>
+      <c r="D3" s="293"/>
+      <c r="E3" s="293"/>
+      <c r="F3" s="293"/>
+      <c r="G3" s="294"/>
     </row>
     <row r="4" spans="1:7" s="99" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="172" t="s">
+      <c r="A4" s="199" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="197"/>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="197"/>
-      <c r="F4" s="197"/>
-      <c r="G4" s="210"/>
+      <c r="B4" s="200"/>
+      <c r="C4" s="200"/>
+      <c r="D4" s="200"/>
+      <c r="E4" s="200"/>
+      <c r="F4" s="200"/>
+      <c r="G4" s="183"/>
     </row>
     <row r="5" spans="1:7" s="99" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="304" t="s">
+      <c r="A5" s="241" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="305"/>
-      <c r="C5" s="305"/>
-      <c r="D5" s="305"/>
-      <c r="E5" s="305"/>
-      <c r="F5" s="305"/>
-      <c r="G5" s="306"/>
+      <c r="B5" s="242"/>
+      <c r="C5" s="242"/>
+      <c r="D5" s="242"/>
+      <c r="E5" s="242"/>
+      <c r="F5" s="242"/>
+      <c r="G5" s="243"/>
     </row>
     <row r="6" spans="1:7" s="99" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="103" t="s">
@@ -6358,14 +6361,14 @@
       <c r="C6" s="105" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="260" t="s">
+      <c r="D6" s="244" t="s">
         <v>142</v>
       </c>
-      <c r="E6" s="262"/>
-      <c r="F6" s="281" t="s">
+      <c r="E6" s="245"/>
+      <c r="F6" s="246" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="285">
+      <c r="G6" s="247">
         <f>Page1!J4</f>
         <v>0</v>
       </c>
@@ -6378,13 +6381,13 @@
       <c r="C7" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="260">
+      <c r="D7" s="244">
         <f>Page1!F5</f>
         <v>0</v>
       </c>
-      <c r="E7" s="262"/>
-      <c r="F7" s="281"/>
-      <c r="G7" s="307"/>
+      <c r="E7" s="245"/>
+      <c r="F7" s="246"/>
+      <c r="G7" s="248"/>
     </row>
     <row r="8" spans="1:7" s="99" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="103" t="s">
@@ -6397,15 +6400,15 @@
       <c r="C8" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="281">
+      <c r="D8" s="246">
         <f>Page1!H5</f>
         <v>0</v>
       </c>
-      <c r="E8" s="281"/>
-      <c r="F8" s="282" t="s">
+      <c r="E8" s="246"/>
+      <c r="F8" s="258" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="285">
+      <c r="G8" s="247">
         <f>Page1!J5</f>
         <v>0</v>
       </c>
@@ -6418,15 +6421,15 @@
         <f>Page1!G44</f>
         <v>461359700</v>
       </c>
-      <c r="C9" s="282" t="s">
+      <c r="C9" s="258" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="288" t="s">
+      <c r="D9" s="263" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="289"/>
-      <c r="F9" s="283"/>
-      <c r="G9" s="286"/>
+      <c r="E9" s="264"/>
+      <c r="F9" s="259"/>
+      <c r="G9" s="261"/>
     </row>
     <row r="10" spans="1:7" s="99" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="110" t="s">
@@ -6436,34 +6439,34 @@
         <f>Page1!C5</f>
         <v>0</v>
       </c>
-      <c r="C10" s="284"/>
-      <c r="D10" s="290"/>
-      <c r="E10" s="291"/>
-      <c r="F10" s="284"/>
-      <c r="G10" s="287"/>
+      <c r="C10" s="260"/>
+      <c r="D10" s="265"/>
+      <c r="E10" s="266"/>
+      <c r="F10" s="260"/>
+      <c r="G10" s="262"/>
     </row>
     <row r="11" spans="1:7" s="99" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="292" t="s">
+      <c r="A11" s="249" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="294" t="s">
+      <c r="B11" s="251" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="296" t="s">
+      <c r="C11" s="253" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="297"/>
-      <c r="E11" s="298"/>
-      <c r="F11" s="294" t="s">
+      <c r="D11" s="254"/>
+      <c r="E11" s="255"/>
+      <c r="F11" s="251" t="s">
         <v>58</v>
       </c>
-      <c r="G11" s="299" t="s">
+      <c r="G11" s="256" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="99" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="293"/>
-      <c r="B12" s="295"/>
+      <c r="A12" s="250"/>
+      <c r="B12" s="252"/>
       <c r="C12" s="112" t="s">
         <v>60</v>
       </c>
@@ -6473,8 +6476,8 @@
       <c r="E12" s="112" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="295"/>
-      <c r="G12" s="300"/>
+      <c r="F12" s="252"/>
+      <c r="G12" s="257"/>
     </row>
     <row r="13" spans="1:7" s="99" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="113" t="s">
@@ -6544,7 +6547,7 @@
         <f>Page1!K39</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G15" s="277" t="s">
+      <c r="G15" s="267" t="s">
         <v>71</v>
       </c>
     </row>
@@ -6568,7 +6571,7 @@
         <f>Page2!F41</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G16" s="228"/>
+      <c r="G16" s="227"/>
     </row>
     <row r="17" spans="1:7" s="99" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="117" t="s">
@@ -6590,7 +6593,7 @@
         <f>Page1!I39</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G17" s="228"/>
+      <c r="G17" s="227"/>
     </row>
     <row r="18" spans="1:7" s="99" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="117" t="s">
@@ -6612,7 +6615,7 @@
         <f>Page2!D41</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" s="228"/>
+      <c r="G18" s="227"/>
     </row>
     <row r="19" spans="1:7" s="99" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="117" t="s">
@@ -6634,7 +6637,7 @@
         <f>Page1!J39</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G19" s="228"/>
+      <c r="G19" s="227"/>
     </row>
     <row r="20" spans="1:7" s="99" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="117" t="s">
@@ -6656,7 +6659,7 @@
         <f>Page2!E41</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G20" s="228"/>
+      <c r="G20" s="227"/>
     </row>
     <row r="21" spans="1:7" s="99" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="117" t="s">
@@ -6678,7 +6681,7 @@
         <f>Page1!G39</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G21" s="228"/>
+      <c r="G21" s="227"/>
     </row>
     <row r="22" spans="1:7" s="99" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="117" t="s">
@@ -6700,7 +6703,7 @@
         <f>Page1!H39</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G22" s="138"/>
+      <c r="G22" s="152"/>
     </row>
     <row r="23" spans="1:7" s="99" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="117" t="s">
@@ -6742,7 +6745,7 @@
       </c>
       <c r="E24" s="39">
         <f>Page2!J9</f>
-        <v>250</v>
+        <v>210</v>
       </c>
       <c r="F24" s="39" t="e">
         <f>Page2!I41</f>
@@ -6800,26 +6803,26 @@
       </c>
     </row>
     <row r="27" spans="1:7" s="99" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="274" t="s">
+      <c r="A27" s="268" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="275"/>
-      <c r="C27" s="275"/>
-      <c r="D27" s="275"/>
-      <c r="E27" s="275"/>
-      <c r="F27" s="275"/>
-      <c r="G27" s="276"/>
+      <c r="B27" s="269"/>
+      <c r="C27" s="269"/>
+      <c r="D27" s="269"/>
+      <c r="E27" s="269"/>
+      <c r="F27" s="269"/>
+      <c r="G27" s="270"/>
     </row>
     <row r="28" spans="1:7" s="99" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="258" t="s">
+      <c r="A28" s="271" t="s">
         <v>91</v>
       </c>
-      <c r="B28" s="259"/>
-      <c r="C28" s="278" t="s">
+      <c r="B28" s="272"/>
+      <c r="C28" s="273" t="s">
         <v>128</v>
       </c>
-      <c r="D28" s="279"/>
-      <c r="E28" s="280"/>
+      <c r="D28" s="274"/>
+      <c r="E28" s="275"/>
       <c r="F28" s="126" t="s">
         <v>92</v>
       </c>
@@ -6828,15 +6831,15 @@
       </c>
     </row>
     <row r="29" spans="1:7" s="99" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="263" t="s">
+      <c r="A29" s="276" t="s">
         <v>94</v>
       </c>
-      <c r="B29" s="262"/>
-      <c r="C29" s="268" t="s">
+      <c r="B29" s="245"/>
+      <c r="C29" s="277" t="s">
         <v>95</v>
       </c>
-      <c r="D29" s="269"/>
-      <c r="E29" s="270"/>
+      <c r="D29" s="278"/>
+      <c r="E29" s="279"/>
       <c r="F29" s="80" t="s">
         <v>92</v>
       </c>
@@ -6845,15 +6848,15 @@
       </c>
     </row>
     <row r="30" spans="1:7" s="99" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="263" t="s">
+      <c r="A30" s="276" t="s">
         <v>96</v>
       </c>
-      <c r="B30" s="262"/>
-      <c r="C30" s="268" t="s">
+      <c r="B30" s="245"/>
+      <c r="C30" s="277" t="s">
         <v>97</v>
       </c>
-      <c r="D30" s="269"/>
-      <c r="E30" s="270"/>
+      <c r="D30" s="278"/>
+      <c r="E30" s="279"/>
       <c r="F30" s="80" t="s">
         <v>92</v>
       </c>
@@ -6862,15 +6865,15 @@
       </c>
     </row>
     <row r="31" spans="1:7" s="99" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="263" t="s">
+      <c r="A31" s="276" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="262"/>
-      <c r="C31" s="268" t="s">
+      <c r="B31" s="245"/>
+      <c r="C31" s="277" t="s">
         <v>99</v>
       </c>
-      <c r="D31" s="269"/>
-      <c r="E31" s="270"/>
+      <c r="D31" s="278"/>
+      <c r="E31" s="279"/>
       <c r="F31" s="80" t="s">
         <v>92</v>
       </c>
@@ -6879,15 +6882,15 @@
       </c>
     </row>
     <row r="32" spans="1:7" s="99" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="263" t="s">
+      <c r="A32" s="276" t="s">
         <v>101</v>
       </c>
-      <c r="B32" s="262"/>
-      <c r="C32" s="268" t="s">
+      <c r="B32" s="245"/>
+      <c r="C32" s="277" t="s">
         <v>102</v>
       </c>
-      <c r="D32" s="269"/>
-      <c r="E32" s="270"/>
+      <c r="D32" s="278"/>
+      <c r="E32" s="279"/>
       <c r="F32" s="80" t="s">
         <v>92</v>
       </c>
@@ -6896,15 +6899,15 @@
       </c>
     </row>
     <row r="33" spans="1:7" s="99" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="263" t="s">
+      <c r="A33" s="276" t="s">
         <v>103</v>
       </c>
-      <c r="B33" s="262"/>
-      <c r="C33" s="268" t="s">
+      <c r="B33" s="245"/>
+      <c r="C33" s="277" t="s">
         <v>104</v>
       </c>
-      <c r="D33" s="269"/>
-      <c r="E33" s="270"/>
+      <c r="D33" s="278"/>
+      <c r="E33" s="279"/>
       <c r="F33" s="80" t="s">
         <v>92</v>
       </c>
@@ -6913,15 +6916,15 @@
       </c>
     </row>
     <row r="34" spans="1:7" s="99" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="152" t="s">
+      <c r="A34" s="143" t="s">
         <v>105</v>
       </c>
-      <c r="B34" s="153"/>
-      <c r="C34" s="271" t="s">
+      <c r="B34" s="144"/>
+      <c r="C34" s="280" t="s">
         <v>106</v>
       </c>
-      <c r="D34" s="272"/>
-      <c r="E34" s="273"/>
+      <c r="D34" s="281"/>
+      <c r="E34" s="282"/>
       <c r="F34" s="127" t="s">
         <v>92</v>
       </c>
@@ -6930,26 +6933,26 @@
       </c>
     </row>
     <row r="35" spans="1:7" s="99" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="274" t="s">
+      <c r="A35" s="268" t="s">
         <v>107</v>
       </c>
-      <c r="B35" s="275"/>
-      <c r="C35" s="275"/>
-      <c r="D35" s="275"/>
-      <c r="E35" s="275"/>
-      <c r="F35" s="275"/>
-      <c r="G35" s="276"/>
+      <c r="B35" s="269"/>
+      <c r="C35" s="269"/>
+      <c r="D35" s="269"/>
+      <c r="E35" s="269"/>
+      <c r="F35" s="269"/>
+      <c r="G35" s="270"/>
     </row>
     <row r="36" spans="1:7" s="99" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="148" t="s">
+      <c r="A36" s="139" t="s">
         <v>108</v>
       </c>
-      <c r="B36" s="149"/>
-      <c r="C36" s="266" t="s">
+      <c r="B36" s="140"/>
+      <c r="C36" s="286" t="s">
         <v>97</v>
       </c>
-      <c r="D36" s="267"/>
-      <c r="E36" s="149"/>
+      <c r="D36" s="287"/>
+      <c r="E36" s="140"/>
       <c r="F36" s="10" t="s">
         <v>92</v>
       </c>
@@ -6958,15 +6961,15 @@
       </c>
     </row>
     <row r="37" spans="1:7" s="99" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="258" t="s">
+      <c r="A37" s="271" t="s">
         <v>109</v>
       </c>
-      <c r="B37" s="259"/>
-      <c r="C37" s="260" t="s">
+      <c r="B37" s="272"/>
+      <c r="C37" s="244" t="s">
         <v>110</v>
       </c>
-      <c r="D37" s="261"/>
-      <c r="E37" s="262"/>
+      <c r="D37" s="283"/>
+      <c r="E37" s="245"/>
       <c r="F37" s="119" t="s">
         <v>92</v>
       </c>
@@ -6975,15 +6978,15 @@
       </c>
     </row>
     <row r="38" spans="1:7" s="99" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="263" t="s">
+      <c r="A38" s="276" t="s">
         <v>111</v>
       </c>
-      <c r="B38" s="262"/>
-      <c r="C38" s="260" t="s">
+      <c r="B38" s="245"/>
+      <c r="C38" s="244" t="s">
         <v>112</v>
       </c>
-      <c r="D38" s="261"/>
-      <c r="E38" s="262"/>
+      <c r="D38" s="283"/>
+      <c r="E38" s="245"/>
       <c r="F38" s="119" t="s">
         <v>92</v>
       </c>
@@ -6992,15 +6995,15 @@
       </c>
     </row>
     <row r="39" spans="1:7" s="99" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="152" t="s">
+      <c r="A39" s="143" t="s">
         <v>113</v>
       </c>
-      <c r="B39" s="153"/>
-      <c r="C39" s="264" t="s">
+      <c r="B39" s="144"/>
+      <c r="C39" s="284" t="s">
         <v>114</v>
       </c>
-      <c r="D39" s="265"/>
-      <c r="E39" s="153"/>
+      <c r="D39" s="285"/>
+      <c r="E39" s="144"/>
       <c r="F39" s="1" t="s">
         <v>92</v>
       </c>
@@ -7009,50 +7012,50 @@
       </c>
     </row>
     <row r="40" spans="1:7" s="99" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="246" t="s">
+      <c r="A40" s="296" t="s">
         <v>115</v>
       </c>
-      <c r="B40" s="247"/>
-      <c r="C40" s="248" t="s">
+      <c r="B40" s="297"/>
+      <c r="C40" s="298" t="s">
         <v>138</v>
       </c>
-      <c r="D40" s="249"/>
-      <c r="E40" s="250"/>
-      <c r="F40" s="248" t="s">
+      <c r="D40" s="299"/>
+      <c r="E40" s="300"/>
+      <c r="F40" s="298" t="s">
         <v>139</v>
       </c>
-      <c r="G40" s="250"/>
+      <c r="G40" s="300"/>
     </row>
     <row r="41" spans="1:7" s="99" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="251"/>
-      <c r="B41" s="252"/>
-      <c r="C41" s="172"/>
-      <c r="D41" s="197"/>
-      <c r="E41" s="210"/>
-      <c r="F41" s="255"/>
-      <c r="G41" s="256"/>
+      <c r="A41" s="301"/>
+      <c r="B41" s="302"/>
+      <c r="C41" s="199"/>
+      <c r="D41" s="200"/>
+      <c r="E41" s="183"/>
+      <c r="F41" s="305"/>
+      <c r="G41" s="306"/>
     </row>
     <row r="42" spans="1:7" s="99" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="253"/>
-      <c r="B42" s="254"/>
-      <c r="C42" s="238" t="s">
+      <c r="A42" s="303"/>
+      <c r="B42" s="304"/>
+      <c r="C42" s="288" t="s">
         <v>22</v>
       </c>
-      <c r="D42" s="257"/>
-      <c r="E42" s="239"/>
-      <c r="F42" s="238" t="s">
+      <c r="D42" s="307"/>
+      <c r="E42" s="289"/>
+      <c r="F42" s="288" t="s">
         <v>140</v>
       </c>
-      <c r="G42" s="239"/>
+      <c r="G42" s="289"/>
     </row>
     <row r="43" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="128"/>
       <c r="B43" s="128"/>
       <c r="C43" s="128"/>
       <c r="D43" s="128"/>
-      <c r="E43" s="245"/>
-      <c r="F43" s="245"/>
-      <c r="G43" s="245"/>
+      <c r="E43" s="295"/>
+      <c r="F43" s="295"/>
+      <c r="G43" s="295"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="46" t="s">
@@ -7061,63 +7064,24 @@
       <c r="B44" s="129"/>
       <c r="C44" s="130"/>
       <c r="D44" s="128"/>
-      <c r="E44" s="240"/>
-      <c r="F44" s="240"/>
-      <c r="G44" s="240"/>
+      <c r="E44" s="290"/>
+      <c r="F44" s="290"/>
+      <c r="G44" s="290"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="241" t="s">
+      <c r="A46" s="291" t="s">
         <v>117</v>
       </c>
-      <c r="B46" s="241"/>
+      <c r="B46" s="291"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="241" t="s">
+      <c r="A47" s="291" t="s">
         <v>118</v>
       </c>
-      <c r="B47" s="241"/>
+      <c r="B47" s="291"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:E10"/>
-    <mergeCell ref="G15:G22"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="A35:G35"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="C36:E36"/>
     <mergeCell ref="F42:G42"/>
     <mergeCell ref="E44:G44"/>
     <mergeCell ref="A46:B46"/>
@@ -7134,6 +7098,45 @@
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="A35:G35"/>
+    <mergeCell ref="G15:G22"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:E10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="79" orientation="portrait" r:id="rId1"/>

</xml_diff>